<commit_message>
Amélioration du portfolio : centrage des projets, suppression du projet vide et de la section Objectifs Professionnels, mise à jour des dates dans le tableau E5, ajout de Tailwind et Bootstrap aux compétences
</commit_message>
<xml_diff>
--- a/public/documents/tbe5.xlsx
+++ b/public/documents/tbe5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kadir\Desktop\portffff\portfff\public\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kadir\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E0EFC2-ADE0-4B7B-AB14-210A60EB5625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F39139F-F6AD-4562-80D4-951C4E60EA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="49">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -101,7 +101,10 @@
     <t>Période (sous la forme du JJ/MM/AA au JJ/MM/AA)</t>
   </si>
   <si>
-    <t>SESSION 2023</t>
+    <t>Réalisations en milieu professionnel en cours de première année</t>
+  </si>
+  <si>
+    <t>Réalisations en milieu professionnel en cours de seconde année</t>
   </si>
   <si>
     <t>x</t>
@@ -141,25 +144,52 @@
     <t>Suivi Agile et mise en production finale dans ServiceNow</t>
   </si>
   <si>
-    <t>Réalisations en milieu professionnel en cours de première année  [Stage]</t>
-  </si>
-  <si>
-    <t>Réalisations en milieu professionnel en cours de seconde année [Alternance]</t>
-  </si>
-  <si>
-    <t>NOM et prénom :  CIFTCI Nicolas Kadir Baran</t>
+    <t>05/10/24 au 12/10/24</t>
+  </si>
+  <si>
+    <t>13/05/2024 au 14/06/2024</t>
+  </si>
+  <si>
+    <t>16/01/2025 au 10/05/2025</t>
+  </si>
+  <si>
+    <t>01/09/2024 au 15/01/2025</t>
+  </si>
+  <si>
+    <t>20/11/24 au 25/11/24</t>
+  </si>
+  <si>
+    <t>02/12/24 au 10/12/24</t>
+  </si>
+  <si>
+    <t>18/01/25 au 24/01/25</t>
+  </si>
+  <si>
+    <t>05/02/25 au 09/02/25</t>
+  </si>
+  <si>
+    <t>15/03/25 au 22/03/25</t>
+  </si>
+  <si>
+    <t>27/03/25 au 31/03/25</t>
+  </si>
+  <si>
+    <t>SESSION 2025</t>
+  </si>
+  <si>
+    <t>☑ SLAM</t>
+  </si>
+  <si>
+    <t>NOM et prénom : CIFTCI Nicolas Kadir Baran</t>
+  </si>
+  <si>
+    <t>Centre de formation : Efrei</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://portfolio-xi-beige-50.vercel.app/</t>
   </si>
   <si>
     <t>N° candidat : 02444876918</t>
-  </si>
-  <si>
-    <t>☑ SLAM</t>
-  </si>
-  <si>
-    <t>Adresse URL du portfolio :https://portfolio-xi-beige-50.vercel.app/</t>
-  </si>
-  <si>
-    <t>Centre de formation : Efrei</t>
   </si>
 </sst>
 </file>
@@ -616,7 +646,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -681,15 +711,39 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -723,28 +777,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1057,70 +1090,70 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E4"/>
+    <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" style="1" customWidth="1"/>
     <col min="3" max="8" width="18.6640625" style="1" customWidth="1"/>
     <col min="9" max="43" width="11.44140625" customWidth="1"/>
     <col min="44" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="43"/>
+      <c r="A3" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="24"/>
+      <c r="H3" s="30"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="A4" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1128,26 +1161,26 @@
         <v>15</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="A5" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="39" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1170,8 +1203,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1227,16 +1260,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1275,24 +1308,26 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="103.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>36</v>
+      </c>
       <c r="C9" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -1332,26 +1367,28 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="103.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="C10" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1391,26 +1428,28 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="C11" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1764,16 +1803,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
+      <c r="A19" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1812,26 +1851,28 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="70.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="C20" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I20"/>
       <c r="J20"/>
@@ -2140,16 +2181,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
+      <c r="A27" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="38"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2188,24 +2229,26 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="C28" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I28"/>
       <c r="J28"/>
@@ -2245,24 +2288,26 @@
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="C29" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I29"/>
       <c r="J29"/>
@@ -2302,24 +2347,26 @@
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="10"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="C30" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I30"/>
       <c r="J30"/>
@@ -2359,24 +2406,26 @@
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="C31" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I31"/>
       <c r="J31"/>
@@ -2416,24 +2465,26 @@
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="C32" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I32"/>
       <c r="J32"/>
@@ -2473,24 +2524,26 @@
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="10"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="C33" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I33"/>
       <c r="J33"/>
@@ -2530,24 +2583,26 @@
     </row>
     <row r="34" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="13"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="C34" s="21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E34" s="19"/>
       <c r="F34" s="21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G34" s="21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I34"/>
       <c r="J34"/>
@@ -2630,15 +2685,27 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:43" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+    </row>
     <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:43" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:43" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="1:43" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:43" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="1:43" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+    </row>
     <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2678,11 +2745,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2690,6 +2752,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>